<commit_message>
Implemented create read update and delete(CRUD)
CRUD implemented
</commit_message>
<xml_diff>
--- a/CMPG323 EcoPower Logistics Data.xlsx
+++ b/CMPG323 EcoPower Logistics Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\code\code\cmpg323\project 4\cmpg323_project4_39909476\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CODE\Code\CMPG323\Project 4\CMPG323_Project4_39909476\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B586C7-8D42-4B93-8E25-CA7B958DE76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C816D267-07DB-49D5-9604-7B820E21E0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="28800" windowHeight="11295" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers" sheetId="1" r:id="rId1"/>
@@ -732,8 +732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,8 +1718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1953,8 +1953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>